<commit_message>
change POSTE en SEGMENT et inscrit l'attribut user (#1)
* change POSTE en SEGMENT et inscrit l'attribut user

* manage error set roles

* disable account management for all users

* first test :)

* mise en place workflow de test

* change le nom du workflow
</commit_message>
<xml_diff>
--- a/userBase.xlsx
+++ b/userBase.xlsx
@@ -35,7 +35,7 @@
     <t xml:space="preserve">ACCES GEOGRAPHIQUE</t>
   </si>
   <si>
-    <t xml:space="preserve">FONCTION</t>
+    <t xml:space="preserve">SEGMENT</t>
   </si>
   <si>
     <t xml:space="preserve">PRENOM</t>
@@ -507,6 +507,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -528,12 +529,14 @@
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -627,10 +630,10 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.96"/>
@@ -708,7 +711,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
@@ -728,11 +731,11 @@
       <selection pane="topLeft" activeCell="A97" activeCellId="0" sqref="A97"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1860,7 +1863,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
feat: modifie le fichier de configuration + sort la conf viper de excel.go
</commit_message>
<xml_diff>
--- a/userBase.xlsx
+++ b/userBase.xlsx
@@ -12,7 +12,7 @@
     <sheet name="zones" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">utilisateurs!$A$1:$I$1144</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">utilisateurs!$A$1:$K$1145</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="174">
   <si>
     <t xml:space="preserve">NIVEAU HABILITATION</t>
   </si>
@@ -35,6 +35,9 @@
     <t xml:space="preserve">ACCES GEOGRAPHIQUE</t>
   </si>
   <si>
+    <t xml:space="preserve">FONCTION</t>
+  </si>
+  <si>
     <t xml:space="preserve">SEGMENT</t>
   </si>
   <si>
@@ -47,12 +50,24 @@
     <t xml:space="preserve">ADRESSE MAIL</t>
   </si>
   <si>
+    <t xml:space="preserve">GOUP</t>
+  </si>
+  <si>
     <t xml:space="preserve">SCOPE</t>
   </si>
   <si>
     <t xml:space="preserve">REGION ADM</t>
   </si>
   <si>
+    <t xml:space="preserve">DOMAINE MAIL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOUBLON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOOKUP</t>
+  </si>
+  <si>
     <t xml:space="preserve">A</t>
   </si>
   <si>
@@ -62,6 +77,9 @@
     <t xml:space="preserve">51</t>
   </si>
   <si>
+    <t xml:space="preserve">Recouvrement et accompagnement des entreprises</t>
+  </si>
+  <si>
     <t xml:space="preserve">LISTENS THE WIND</t>
   </si>
   <si>
@@ -78,6 +96,42 @@
   </si>
   <si>
     <t xml:space="preserve">Nevada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zone51.gov.fr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SIGNAUX FAIBLES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">France entière</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Développeur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raphaël</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SQUELBUT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">raphael.squelbut@shodo.io</t>
+  </si>
+  <si>
+    <t xml:space="preserve">signauxfaibles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wekan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SYSTEME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kcadmin</t>
   </si>
   <si>
     <t xml:space="preserve">REGION</t>
@@ -502,7 +556,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -532,6 +586,12 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
@@ -547,12 +607,19 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
@@ -581,7 +648,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -602,7 +669,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -615,6 +690,22 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="00FFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF0000FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
 </styleSheet>
 </file>
 
@@ -627,23 +718,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="8.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="38.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="22.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="38.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="24.41"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="38.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="38.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="22.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="38.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="10.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="24.41"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -656,7 +748,7 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
@@ -674,47 +766,141 @@
       <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="F2" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="4"/>
+      <c r="J2" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="M2" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" s="0" t="s">
-        <v>17</v>
+      <c r="B3" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="L3" s="5" t="str">
+        <f aca="false">RIGHT(H3,LEN(H3)-FIND("@",H3,1))</f>
+        <v>shodo.io</v>
+      </c>
+      <c r="M3" s="5" t="n">
+        <f aca="false">COUNTIF( H:H, H3)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5" t="n">
+        <f aca="false">COUNTIF( H:H, H4)</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I1144"/>
+  <autoFilter ref="A1:K1145"/>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" display="john.doe@zone51.gov.fr"/>
+    <hyperlink ref="H2" r:id="rId1" display="john.doe@zone51.gov.fr"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
   <drawing r:id="rId2"/>
 </worksheet>
@@ -727,11 +913,11 @@
   </sheetPr>
   <dimension ref="A1:C102"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A97" activeCellId="0" sqref="A97"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.36"/>
@@ -739,1125 +925,1125 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>20</v>
+      <c r="A1" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>48</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>49</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>50</v>
+        <v>68</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>51</v>
+        <v>69</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>52</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>50</v>
+        <v>68</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>51</v>
+        <v>69</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>53</v>
+        <v>71</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>50</v>
+        <v>68</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>51</v>
+        <v>69</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>54</v>
+        <v>72</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>50</v>
+        <v>68</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>51</v>
+        <v>69</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>55</v>
+        <v>73</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>50</v>
+        <v>68</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>57</v>
+        <v>75</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>50</v>
+        <v>68</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>50</v>
+        <v>68</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>50</v>
+        <v>68</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>50</v>
+        <v>68</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>50</v>
+        <v>68</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>62</v>
+        <v>80</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>50</v>
+        <v>68</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>63</v>
+        <v>81</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>50</v>
+        <v>68</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>67</v>
+        <v>85</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>68</v>
+        <v>86</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>69</v>
+        <v>87</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>70</v>
+        <v>88</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>71</v>
+        <v>89</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>70</v>
+        <v>88</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>72</v>
+        <v>90</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>73</v>
+        <v>91</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>74</v>
+        <v>92</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>75</v>
+        <v>93</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>73</v>
+        <v>91</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>74</v>
+        <v>92</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>76</v>
+        <v>94</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>73</v>
+        <v>91</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>74</v>
+        <v>92</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>77</v>
+        <v>95</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>73</v>
+        <v>91</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>74</v>
+        <v>92</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>78</v>
+        <v>96</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>73</v>
+        <v>91</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>79</v>
+        <v>97</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>80</v>
+        <v>98</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>73</v>
+        <v>91</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>79</v>
+        <v>97</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>81</v>
+        <v>99</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>73</v>
+        <v>91</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>79</v>
+        <v>97</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>82</v>
+        <v>100</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>73</v>
+        <v>91</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>79</v>
+        <v>97</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>83</v>
+        <v>101</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>84</v>
+        <v>102</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>84</v>
+        <v>102</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>85</v>
+        <v>103</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>84</v>
+        <v>102</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>84</v>
+        <v>102</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>86</v>
+        <v>104</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>84</v>
+        <v>102</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>84</v>
+        <v>102</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>87</v>
+        <v>105</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>84</v>
+        <v>102</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>84</v>
+        <v>102</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>88</v>
+        <v>106</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>89</v>
+        <v>107</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>90</v>
+        <v>108</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>91</v>
+        <v>109</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>89</v>
+        <v>107</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>90</v>
+        <v>108</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>92</v>
+        <v>110</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>89</v>
+        <v>107</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>90</v>
+        <v>108</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>93</v>
+        <v>111</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>89</v>
+        <v>107</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>90</v>
+        <v>108</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>94</v>
+        <v>112</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>89</v>
+        <v>107</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>90</v>
+        <v>108</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>95</v>
+        <v>113</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>89</v>
+        <v>107</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>90</v>
+        <v>108</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>96</v>
+        <v>114</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>98</v>
+        <v>116</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>99</v>
+        <v>117</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>100</v>
+        <v>118</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>100</v>
+        <v>118</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>101</v>
+        <v>119</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>102</v>
+        <v>120</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>102</v>
+        <v>120</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>103</v>
+        <v>121</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>104</v>
+        <v>122</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>104</v>
+        <v>122</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>105</v>
+        <v>123</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>106</v>
+        <v>124</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>106</v>
+        <v>124</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>107</v>
+        <v>125</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>108</v>
+        <v>126</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>108</v>
+        <v>126</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>109</v>
+        <v>127</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>110</v>
+        <v>128</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>110</v>
+        <v>128</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>111</v>
+        <v>129</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>110</v>
+        <v>128</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>110</v>
+        <v>128</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>112</v>
+        <v>130</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>110</v>
+        <v>128</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>110</v>
+        <v>128</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>113</v>
+        <v>131</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>110</v>
+        <v>128</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>110</v>
+        <v>128</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>114</v>
+        <v>132</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>110</v>
+        <v>128</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>110</v>
+        <v>128</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>115</v>
+        <v>133</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>110</v>
+        <v>128</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>110</v>
+        <v>128</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>116</v>
+        <v>134</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>110</v>
+        <v>128</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>110</v>
+        <v>128</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>117</v>
+        <v>135</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>110</v>
+        <v>128</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>110</v>
+        <v>128</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>119</v>
+        <v>137</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>120</v>
+        <v>138</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>121</v>
+        <v>139</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>119</v>
+        <v>137</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>120</v>
+        <v>138</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>122</v>
+        <v>140</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>119</v>
+        <v>137</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>120</v>
+        <v>138</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>123</v>
+        <v>141</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>119</v>
+        <v>137</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>120</v>
+        <v>138</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>124</v>
+        <v>142</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>119</v>
+        <v>137</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>120</v>
+        <v>138</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>125</v>
+        <v>143</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>119</v>
+        <v>137</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>126</v>
+        <v>144</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>127</v>
+        <v>145</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>119</v>
+        <v>137</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>126</v>
+        <v>144</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>128</v>
+        <v>146</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>119</v>
+        <v>137</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>126</v>
+        <v>144</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>129</v>
+        <v>147</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>119</v>
+        <v>137</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>126</v>
+        <v>144</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>130</v>
+        <v>148</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>119</v>
+        <v>137</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>126</v>
+        <v>144</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>131</v>
+        <v>149</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>119</v>
+        <v>137</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>126</v>
+        <v>144</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>132</v>
+        <v>150</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>119</v>
+        <v>137</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>126</v>
+        <v>144</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>133</v>
+        <v>151</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>119</v>
+        <v>137</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>126</v>
+        <v>144</v>
       </c>
       <c r="C86" s="0" t="s">
-        <v>134</v>
+        <v>152</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>135</v>
+        <v>153</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>136</v>
+        <v>154</v>
       </c>
       <c r="C87" s="0" t="s">
-        <v>137</v>
+        <v>155</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>135</v>
+        <v>153</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>136</v>
+        <v>154</v>
       </c>
       <c r="C88" s="0" t="s">
-        <v>138</v>
+        <v>156</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>135</v>
+        <v>153</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>139</v>
+        <v>157</v>
       </c>
       <c r="C89" s="0" t="s">
-        <v>140</v>
+        <v>158</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>135</v>
+        <v>153</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>139</v>
+        <v>157</v>
       </c>
       <c r="C90" s="0" t="s">
-        <v>141</v>
+        <v>159</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>135</v>
+        <v>153</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>139</v>
+        <v>157</v>
       </c>
       <c r="C91" s="0" t="s">
-        <v>142</v>
+        <v>160</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>143</v>
+        <v>161</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>143</v>
+        <v>161</v>
       </c>
       <c r="C92" s="0" t="s">
-        <v>144</v>
+        <v>162</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>143</v>
+        <v>161</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>143</v>
+        <v>161</v>
       </c>
       <c r="C93" s="0" t="s">
-        <v>145</v>
+        <v>163</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>143</v>
+        <v>161</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>143</v>
+        <v>161</v>
       </c>
       <c r="C94" s="0" t="s">
-        <v>146</v>
+        <v>164</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>143</v>
+        <v>161</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>143</v>
+        <v>161</v>
       </c>
       <c r="C95" s="0" t="s">
-        <v>147</v>
+        <v>165</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>143</v>
+        <v>161</v>
       </c>
       <c r="B96" s="0" t="s">
-        <v>143</v>
+        <v>161</v>
       </c>
       <c r="C96" s="0" t="s">
-        <v>148</v>
+        <v>166</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>149</v>
+        <v>167</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>149</v>
+        <v>167</v>
       </c>
       <c r="C97" s="0" t="s">
-        <v>150</v>
+        <v>168</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A98" s="2" t="s">
-        <v>149</v>
+        <v>167</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>149</v>
+        <v>167</v>
       </c>
       <c r="C98" s="0" t="s">
-        <v>151</v>
+        <v>169</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A99" s="2" t="s">
-        <v>149</v>
+        <v>167</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>149</v>
+        <v>167</v>
       </c>
       <c r="C99" s="0" t="s">
-        <v>152</v>
+        <v>170</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A100" s="2" t="s">
-        <v>149</v>
+        <v>167</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>149</v>
+        <v>167</v>
       </c>
       <c r="C100" s="0" t="s">
-        <v>153</v>
+        <v>171</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A101" s="2" t="s">
-        <v>149</v>
+        <v>167</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>149</v>
+        <v>167</v>
       </c>
       <c r="C101" s="0" t="s">
-        <v>154</v>
+        <v>172</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A102" s="2" t="s">
-        <v>149</v>
+        <v>167</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>149</v>
+        <v>167</v>
       </c>
       <c r="C102" s="0" t="s">
-        <v>155</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -1865,8 +2051,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
now test is working
</commit_message>
<xml_diff>
--- a/userBase.xlsx
+++ b/userBase.xlsx
@@ -12,7 +12,7 @@
     <sheet name="zones" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">utilisateurs!$A$1:$K$1145</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">utilisateurs!$A$1:$K$1146</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="179">
   <si>
     <t xml:space="preserve">NIVEAU HABILITATION</t>
   </si>
@@ -59,13 +59,13 @@
     <t xml:space="preserve">REGION ADM</t>
   </si>
   <si>
+    <t xml:space="preserve">BOARDS</t>
+  </si>
+  <si>
     <t xml:space="preserve">DOMAINE MAIL</t>
   </si>
   <si>
-    <t xml:space="preserve">DOUBLON</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOOKUP</t>
+    <t xml:space="preserve">DOUBLON LOOKUP</t>
   </si>
   <si>
     <t xml:space="preserve">A</t>
@@ -126,6 +126,21 @@
   </si>
   <si>
     <t xml:space="preserve">wekan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tableau-crp-bfc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Herbert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LEONARD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">herbert.leonard@pantheon.fr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tableau-crp-bfc,tableau-codefi-nord</t>
   </si>
   <si>
     <t xml:space="preserve">SYSTEME</t>
@@ -718,13 +733,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.96"/>
@@ -736,6 +751,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="38.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="10.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="24.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="34.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="14.73"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -772,7 +789,7 @@
       <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
       <c r="M1" s="0" t="s">
@@ -814,10 +831,10 @@
       <c r="K2" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="0" t="s">
+      <c r="M2" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="M2" s="0" t="n">
+      <c r="N2" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -855,43 +872,91 @@
       <c r="K3" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="L3" s="5" t="str">
+      <c r="L3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="M3" s="5" t="str">
         <f aca="false">RIGHT(H3,LEN(H3)-FIND("@",H3,1))</f>
         <v>shodo.io</v>
       </c>
-      <c r="M3" s="5" t="n">
+      <c r="N3" s="5" t="n">
         <f aca="false">COUNTIF( H:H, H3)</f>
         <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="n">
-        <v>0</v>
+      <c r="A4" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
+        <v>25</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="F4" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="G4" s="5"/>
+      <c r="G4" s="5" t="s">
+        <v>36</v>
+      </c>
       <c r="H4" s="5" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5" t="n">
+      <c r="J4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M4" s="5" t="str">
+        <f aca="false">RIGHT(H4,LEN(H4)-FIND("@",H4,1))</f>
+        <v>pantheon.fr</v>
+      </c>
+      <c r="N4" s="5" t="n">
         <f aca="false">COUNTIF( H:H, H4)</f>
         <v>1</v>
       </c>
     </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5" t="n">
+        <f aca="false">COUNTIF( H:H, H5)</f>
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:K1145"/>
+  <autoFilter ref="A1:K1146"/>
   <hyperlinks>
     <hyperlink ref="H2" r:id="rId1" display="john.doe@zone51.gov.fr"/>
   </hyperlinks>
@@ -899,8 +964,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
   <drawing r:id="rId2"/>
 </worksheet>
@@ -917,7 +982,7 @@
       <selection pane="topLeft" activeCell="A97" activeCellId="0" sqref="A97"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.36"/>
@@ -926,65 +991,65 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>16</v>
@@ -992,1058 +1057,1058 @@
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="C86" s="0" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="C87" s="0" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="C88" s="0" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="C89" s="0" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="C90" s="0" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="C91" s="0" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="C92" s="0" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="C93" s="0" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="C94" s="0" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="C95" s="0" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="B96" s="0" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="C96" s="0" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="C97" s="0" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A98" s="2" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="C98" s="0" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A99" s="2" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="C99" s="0" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A100" s="2" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="C100" s="0" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A101" s="2" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="C101" s="0" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A102" s="2" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="C102" s="0" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -2051,8 +2116,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
UpdateAll() -> UpdateKeycloak() + fix tests
</commit_message>
<xml_diff>
--- a/userBase.xlsx
+++ b/userBase.xlsx
@@ -12,7 +12,7 @@
     <sheet name="zones" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">utilisateurs!$A$1:$K$1146</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">utilisateurs!$A$1:$L$1145</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="177">
   <si>
     <t xml:space="preserve">NIVEAU HABILITATION</t>
   </si>
@@ -56,6 +56,9 @@
     <t xml:space="preserve">SCOPE</t>
   </si>
   <si>
+    <t xml:space="preserve">TASKFORCE</t>
+  </si>
+  <si>
     <t xml:space="preserve">REGION ADM</t>
   </si>
   <si>
@@ -128,19 +131,10 @@
     <t xml:space="preserve">wekan</t>
   </si>
   <si>
+    <t xml:space="preserve">labelle_bleue</t>
+  </si>
+  <si>
     <t xml:space="preserve">tableau-crp-bfc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Herbert</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LEONARD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">herbert.leonard@pantheon.fr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tableau-crp-bfc,tableau-codefi-nord</t>
   </si>
   <si>
     <t xml:space="preserve">SYSTEME</t>
@@ -733,26 +727,26 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K3" activeCellId="0" sqref="K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.96"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="38.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="38.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="22.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="38.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="10.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="24.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="34.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="14.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="0" width="24.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="34.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="14.73"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -792,171 +786,134 @@
       <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
       <c r="N1" s="0" t="s">
         <v>13</v>
       </c>
+      <c r="O1" s="0" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I2" s="4"/>
       <c r="J2" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="K2" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="M2" s="0" t="s">
+      <c r="L2" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="N2" s="0" t="n">
+      <c r="N2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="O2" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D3" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L3" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="M3" s="5" t="str">
+      <c r="M3" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="N3" s="5" t="str">
         <f aca="false">RIGHT(H3,LEN(H3)-FIND("@",H3,1))</f>
         <v>shodo.io</v>
       </c>
-      <c r="N3" s="5" t="n">
+      <c r="O3" s="5" t="n">
         <f aca="false">COUNTIF( H:H, H3)</f>
         <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
-        <v>14</v>
+      <c r="A4" s="5" t="n">
+        <v>0</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>28</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
       <c r="F4" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>36</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="G4" s="5"/>
       <c r="H4" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I4" s="5"/>
-      <c r="J4" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="L4" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="M4" s="5" t="str">
-        <f aca="false">RIGHT(H4,LEN(H4)-FIND("@",H4,1))</f>
-        <v>pantheon.fr</v>
-      </c>
-      <c r="N4" s="5" t="n">
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5" t="n">
         <f aca="false">COUNTIF( H:H, H4)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5" t="n">
-        <f aca="false">COUNTIF( H:H, H5)</f>
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:K1146"/>
+  <autoFilter ref="A1:L1145"/>
   <hyperlinks>
     <hyperlink ref="H2" r:id="rId1" display="john.doe@zone51.gov.fr"/>
   </hyperlinks>
@@ -982,7 +939,7 @@
       <selection pane="topLeft" activeCell="A97" activeCellId="0" sqref="A97"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.36"/>
@@ -991,1124 +948,1124 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>41</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="0" t="s">
         <v>44</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>45</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B5" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="0" t="s">
         <v>48</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B9" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="0" t="s">
         <v>52</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" s="0" t="s">
         <v>57</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B13" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" s="0" t="s">
         <v>58</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B18" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" s="0" t="s">
         <v>64</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B21" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="C21" s="0" t="s">
         <v>68</v>
-      </c>
-      <c r="C21" s="0" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C24" s="0" t="s">
         <v>73</v>
-      </c>
-      <c r="B24" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="C24" s="0" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B25" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C25" s="0" t="s">
         <v>74</v>
-      </c>
-      <c r="C25" s="0" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B29" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="C29" s="0" t="s">
         <v>79</v>
-      </c>
-      <c r="C29" s="0" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="C36" s="0" t="s">
         <v>88</v>
-      </c>
-      <c r="B36" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="C36" s="0" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B37" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="C37" s="0" t="s">
         <v>89</v>
-      </c>
-      <c r="C37" s="0" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B40" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C40" s="0" t="s">
         <v>93</v>
-      </c>
-      <c r="C40" s="0" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="C41" s="0" t="s">
         <v>96</v>
-      </c>
-      <c r="B41" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="C41" s="0" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B42" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="C42" s="0" t="s">
         <v>97</v>
-      </c>
-      <c r="C42" s="0" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B46" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C46" s="0" t="s">
         <v>102</v>
-      </c>
-      <c r="C46" s="0" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="B50" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="C50" s="0" t="s">
         <v>107</v>
-      </c>
-      <c r="B50" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="C50" s="0" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="B53" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="C53" s="0" t="s">
         <v>112</v>
-      </c>
-      <c r="B53" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="C53" s="0" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B54" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C54" s="0" t="s">
         <v>113</v>
-      </c>
-      <c r="C54" s="0" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="B60" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="C60" s="0" t="s">
         <v>120</v>
-      </c>
-      <c r="B60" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="C60" s="0" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="B67" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="C67" s="0" t="s">
         <v>133</v>
-      </c>
-      <c r="B67" s="0" t="s">
-        <v>133</v>
-      </c>
-      <c r="C67" s="0" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="B74" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="C74" s="0" t="s">
         <v>142</v>
-      </c>
-      <c r="B74" s="0" t="s">
-        <v>143</v>
-      </c>
-      <c r="C74" s="0" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B75" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="C75" s="0" t="s">
         <v>143</v>
-      </c>
-      <c r="C75" s="0" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B80" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="C80" s="0" t="s">
         <v>149</v>
-      </c>
-      <c r="C80" s="0" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C86" s="0" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="B87" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="C87" s="0" t="s">
         <v>158</v>
-      </c>
-      <c r="B87" s="0" t="s">
-        <v>159</v>
-      </c>
-      <c r="C87" s="0" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B88" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="C88" s="0" t="s">
         <v>159</v>
-      </c>
-      <c r="C88" s="0" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C89" s="0" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B90" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="C90" s="0" t="s">
         <v>162</v>
-      </c>
-      <c r="C90" s="0" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C91" s="0" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C92" s="0" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="B93" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="C93" s="0" t="s">
         <v>166</v>
-      </c>
-      <c r="B93" s="0" t="s">
-        <v>166</v>
-      </c>
-      <c r="C93" s="0" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C94" s="0" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C95" s="0" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B96" s="0" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C96" s="0" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C97" s="0" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A98" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C98" s="0" t="s">
         <v>172</v>
-      </c>
-      <c r="B98" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="C98" s="0" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A99" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C99" s="0" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A100" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C100" s="0" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A101" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C101" s="0" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A102" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C102" s="0" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>

</xml_diff>